<commit_message>
Added SpikeList Output Variable
added the SpikeList output variable.

This is a vector of vectors with each vector representing the set of
spikes that are scheduled to arrive at the time instant next to the one
reffered to bby the position of the vector.

It has a special output code that outputs QueueSize-1 extra vectors more
than the number of time slots in order to take account of spikes that
have been generated but are not to be processed in the iteration after
the last.

Also, SpikeList output is only done in case of Full Output as that is
the only case where it makes sense.
</commit_message>
<xml_diff>
--- a/TimeDelNetSimMEX_Lib/Items/enumedit.xlsx
+++ b/TimeDelNetSimMEX_Lib/Items/enumedit.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>V_REQ</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>I_IN_REQ</t>
+  </si>
+  <si>
+    <t>SPIKE_LIST_REQ</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
         <v xml:space="preserve">V_REQ               = (1 &lt;&lt; 0), </v>
       </c>
       <c r="G2">
-        <f>MAX(C2:C17)</f>
+        <f>MAX(C2:C18)</f>
         <v>18</v>
       </c>
     </row>
@@ -476,15 +479,15 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" si="0">LEN(A3)</f>
+        <f t="shared" ref="C3:C18" si="0">LEN(A3)</f>
         <v>10</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D17" si="1">CONCATENATE(A3, REPT(" ",$G$2+1-C3))</f>
+        <f t="shared" ref="D3:D18" si="1">CONCATENATE(A3, REPT(" ",$G$2+1-C3))</f>
         <v xml:space="preserve">I_IN_1_REQ         </v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E17" si="2">CONCATENATE(D3," = (1 &lt;&lt; ",B3,"), ")</f>
+        <f t="shared" ref="E3:E18" si="2">CONCATENATE(D3," = (1 &lt;&lt; ",B3,"), ")</f>
         <v xml:space="preserve">I_IN_1_REQ          = (1 &lt;&lt; 1), </v>
       </c>
     </row>
@@ -730,42 +733,62 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">INITIAL_STATE_REQ  </v>
+        <v xml:space="preserve">SPIKE_LIST_REQ     </v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">INITIAL_STATE_REQ   = (1 &lt;&lt; 14), </v>
+        <v xml:space="preserve">SPIKE_LIST_REQ      = (1 &lt;&lt; 14), </v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">INITIAL_STATE_REQ  </v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">INITIAL_STATE_REQ   = (1 &lt;&lt; 15), </v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D18" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">FINAL_STATE_REQ    </v>
       </c>
-      <c r="E17" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">FINAL_STATE_REQ     = (1 &lt;&lt; 15), </v>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">FINAL_STATE_REQ     = (1 &lt;&lt; 16), </v>
       </c>
     </row>
   </sheetData>

</xml_diff>